<commit_message>
adds metadata needed to run xml and fills in make metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_catch_metadata.xlsx
+++ b/data-raw/metadata/yuba_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-yuba-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-yuba-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937764E3-08C8-3F4F-9FA2-5D1DC4F06EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015EBDE3-4506-F048-9656-897AF0A507E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60140" yWindow="640" windowWidth="37180" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Yuba River RST program</t>
-  </si>
-  <si>
-    <t>projectDescriptionID</t>
   </si>
 </sst>
 </file>
@@ -541,9 +538,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28833,8 +28830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28887,7 +28884,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
updates metadata to remove columns
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_catch_metadata.xlsx
+++ b/data-raw/metadata/yuba_catch_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-yuba-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015EBDE3-4506-F048-9656-897AF0A507E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E4567-31E8-104C-BC7A-F7EF693F2C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60140" yWindow="640" windowWidth="37180" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -184,9 +184,6 @@
     <t>lifeStage</t>
   </si>
   <si>
-    <t>mort</t>
-  </si>
-  <si>
     <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 7.</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
   </si>
   <si>
     <t>Life stage of the fish. Levels = c("Not recorded", "Parr", "Smolt", "Silvery parr", "Fry", "Ammocoete", "Yolk sac fry (alevin)")</t>
-  </si>
-  <si>
-    <t>Whether or not the fish was alive. Levels = c("No", "Yes")</t>
   </si>
   <si>
     <t>Whether the count (n) is an actual count or estimate. Levels = "Yes"</t>
@@ -536,11 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -619,7 +613,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -739,7 +733,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -777,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -815,7 +809,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -891,7 +885,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -967,7 +961,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1005,7 +999,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1043,7 +1037,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1078,28 +1072,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="13">
+        <v>11</v>
+      </c>
+      <c r="M14" s="13">
+        <v>550</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1116,10 +1120,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
@@ -1137,16 +1141,16 @@
         <v>47</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="13">
-        <v>11</v>
+        <v>1</v>
       </c>
-      <c r="M15" s="13">
-        <v>550</v>
+      <c r="M15" s="3">
+        <v>510</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1164,10 +1168,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
@@ -1182,19 +1186,19 @@
         <v>25</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
       <c r="L16" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="3">
-        <v>510</v>
+        <v>195</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1212,38 +1216,28 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="2"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="13">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3">
-        <v>195</v>
-      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="3"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1259,28 +1253,18 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1380,9 +1364,8 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -1408,8 +1391,9 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
@@ -1577,34 +1561,34 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1636,39 +1620,29 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1687,6 +1661,16 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1817,7 +1801,6 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1845,6 +1828,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1872,7 +1856,6 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1900,6 +1883,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2851,7 +2835,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
+      <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
@@ -28778,46 +28762,18 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
-    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1001" s="1"/>
-      <c r="B1001" s="1"/>
-      <c r="C1001" s="1"/>
-      <c r="D1001" s="2"/>
-      <c r="E1001" s="1"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="2"/>
-      <c r="J1001" s="3"/>
-      <c r="K1001" s="2"/>
-      <c r="L1001" s="3"/>
-      <c r="M1001" s="3"/>
-      <c r="N1001" s="1"/>
-      <c r="O1001" s="1"/>
-      <c r="P1001" s="1"/>
-      <c r="Q1001" s="1"/>
-      <c r="R1001" s="1"/>
-      <c r="S1001" s="1"/>
-      <c r="T1001" s="1"/>
-      <c r="U1001" s="1"/>
-      <c r="V1001" s="1"/>
-      <c r="W1001" s="1"/>
-      <c r="X1001" s="1"/>
-      <c r="Y1001" s="1"/>
-      <c r="Z1001" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C1:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C57:C1000 C33:C45 C1:C31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E1:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E33:E1000 E1:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F1:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F33:F1000 F1:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H1:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33:H1000 H1:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28881,7 +28837,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
merges main and updates historic data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_catch_metadata.xlsx
+++ b/data-raw/metadata/yuba_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-yuba-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015EBDE3-4506-F048-9656-897AF0A507E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B2291A-FA2D-5E4A-96E9-312D3697EE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60140" yWindow="640" windowWidth="37180" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="500" windowWidth="34340" windowHeight="27040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -184,9 +184,6 @@
     <t>lifeStage</t>
   </si>
   <si>
-    <t>mort</t>
-  </si>
-  <si>
     <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 7.</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
   </si>
   <si>
     <t>Life stage of the fish. Levels = c("Not recorded", "Parr", "Smolt", "Silvery parr", "Fry", "Ammocoete", "Yolk sac fry (alevin)")</t>
-  </si>
-  <si>
-    <t>Whether or not the fish was alive. Levels = c("No", "Yes")</t>
   </si>
   <si>
     <t>Whether the count (n) is an actual count or estimate. Levels = "Yes"</t>
@@ -536,11 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -619,7 +613,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -715,7 +709,7 @@
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="12">
-        <v>44851.582453703704</v>
+        <v>36489</v>
       </c>
       <c r="M4" s="12">
         <v>45133.427314814813</v>
@@ -739,7 +733,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -777,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -815,7 +809,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -891,7 +885,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -967,7 +961,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1005,7 +999,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1043,7 +1037,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1078,28 +1072,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="13">
+        <v>1</v>
+      </c>
+      <c r="M14" s="13">
+        <v>723</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1116,10 +1120,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
@@ -1137,16 +1141,16 @@
         <v>47</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="13">
-        <v>11</v>
+        <v>1</v>
       </c>
-      <c r="M15" s="13">
-        <v>550</v>
+      <c r="M15" s="3">
+        <v>510</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1164,10 +1168,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
@@ -1182,19 +1186,19 @@
         <v>25</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
       <c r="L16" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="3">
-        <v>510</v>
+        <v>85007</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1212,38 +1216,28 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="2"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="13">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3">
-        <v>195</v>
-      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="3"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1259,28 +1253,18 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1380,9 +1364,8 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -1408,8 +1391,9 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
@@ -1577,34 +1561,34 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1636,39 +1620,29 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1687,6 +1661,16 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1817,7 +1801,6 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1845,6 +1828,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1872,7 +1856,6 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1900,6 +1883,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2851,7 +2835,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
+      <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
@@ -28778,46 +28762,18 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
-    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1001" s="1"/>
-      <c r="B1001" s="1"/>
-      <c r="C1001" s="1"/>
-      <c r="D1001" s="2"/>
-      <c r="E1001" s="1"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="2"/>
-      <c r="J1001" s="3"/>
-      <c r="K1001" s="2"/>
-      <c r="L1001" s="3"/>
-      <c r="M1001" s="3"/>
-      <c r="N1001" s="1"/>
-      <c r="O1001" s="1"/>
-      <c r="P1001" s="1"/>
-      <c r="Q1001" s="1"/>
-      <c r="R1001" s="1"/>
-      <c r="S1001" s="1"/>
-      <c r="T1001" s="1"/>
-      <c r="U1001" s="1"/>
-      <c r="V1001" s="1"/>
-      <c r="W1001" s="1"/>
-      <c r="X1001" s="1"/>
-      <c r="Y1001" s="1"/>
-      <c r="Z1001" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C1:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C57:C1000 C33:C45 C1:C31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E1:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E33:E1000 E1:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F1:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F33:F1000 F1:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H1:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33:H1000 H1:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28881,7 +28837,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
update methods with caveat about run
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_catch_metadata.xlsx
+++ b/data-raw/metadata/yuba_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-yuba-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B2291A-FA2D-5E4A-96E9-312D3697EE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07E61BE-FD95-884A-AA45-152DA6841D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="500" windowWidth="34340" windowHeight="27040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="500" windowWidth="39380" windowHeight="26620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>Common name of species. Levels =c("Chinook salmon", "Steelhead / rainbow trout", "Riffle sculpin",  "Smallmouth bass", "Bluegill", "Pacific lamprey", "Sacramento sucker",  "Mosquitofish", "Not applicable (n/a)", "Sacramento pikeminnow",  "Wakasagi / Japanese smelt", "Hardhead", "Unknown lamprey (Entosphenus or Lampetra)",  "Unknown bass (Micropterus)", "Speckled dace", "Green sunfish",  "Unknown sunfish (Lepomis)", "Prickly sculpin", "Largemouth bass",  "Golden shiner", "Unknown sculpin (Cottus)", "Channel catfish",  "Spotted bass", "River lamprey", "White crappie", "Tule perch",  "Redear sunfish", "Sacramento perch", "Unknown minnow", "Other",  "Unknown Lampetra", "Goldfish", "American shad")</t>
   </si>
   <si>
-    <t>Run designation as determined in the field or as assigned at a later date.  Levels = c("Not recorded", "Spring", "Fall", "Winter", "Late fall")</t>
-  </si>
-  <si>
     <t>Origin/production type of the fish. Levels = c("Natural", "Hatchery")</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Yuba River RST program</t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date. Run assignments in the historical data may be inconsistent with contemporary methods for assigning run. Levels = c("Not recorded", "Spring", "Fall", "Winter", "Late fall")</t>
   </si>
 </sst>
 </file>
@@ -532,9 +532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -961,7 +961,7 @@
         <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -999,7 +999,7 @@
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1037,7 +1037,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1219,7 +1219,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -28837,7 +28837,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
updates metadata to reflect changes in data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_catch_metadata.xlsx
+++ b/data-raw/metadata/yuba_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-yuba-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07E61BE-FD95-884A-AA45-152DA6841D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7C918E-0943-0942-BD89-26E844FC5853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="500" windowWidth="39380" windowHeight="26620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="600" windowWidth="32220" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -89,12 +89,6 @@
   </si>
   <si>
     <t>Foreign key to the CAMP TrapVisit table</t>
-  </si>
-  <si>
-    <t>releaseID</t>
-  </si>
-  <si>
-    <t>Foreign Key to the CAMP Release table</t>
   </si>
   <si>
     <t>forkLength</t>
@@ -530,11 +524,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -610,10 +604,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -622,7 +616,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -686,26 +680,26 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="12">
@@ -730,10 +724,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -768,10 +762,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -806,10 +800,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -882,10 +876,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -920,13 +914,13 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
@@ -958,10 +952,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -996,10 +990,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1034,28 +1028,38 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="3"/>
+      <c r="L13" s="13">
+        <v>1</v>
+      </c>
+      <c r="M13" s="13">
+        <v>723</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1072,28 +1076,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
@@ -1101,8 +1105,8 @@
       <c r="L14" s="13">
         <v>1</v>
       </c>
-      <c r="M14" s="13">
-        <v>723</v>
+      <c r="M14" s="3">
+        <v>510</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1126,31 +1130,31 @@
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="3">
-        <v>510</v>
+        <v>85007</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1168,38 +1172,28 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="13">
-        <v>0</v>
-      </c>
-      <c r="M16" s="3">
-        <v>85007</v>
-      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="3"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1215,28 +1209,18 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="7"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1336,9 +1320,8 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
@@ -1364,8 +1347,9 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -1533,34 +1517,34 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
+      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
@@ -1592,39 +1576,29 @@
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-      <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-      <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-      <c r="X30" s="4"/>
-      <c r="Y30" s="4"/>
-      <c r="Z30" s="4"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
       <c r="K31" s="2"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -1643,6 +1617,16 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1773,7 +1757,6 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1801,6 +1784,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1828,7 +1812,6 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1856,6 +1839,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -2807,7 +2791,7 @@
       <c r="Z73" s="1"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
+      <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="2"/>
@@ -28734,46 +28718,18 @@
       <c r="Y999" s="1"/>
       <c r="Z999" s="1"/>
     </row>
-    <row r="1000" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="1"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="3"/>
-      <c r="G1000" s="3"/>
-      <c r="H1000" s="3"/>
-      <c r="I1000" s="2"/>
-      <c r="J1000" s="3"/>
-      <c r="K1000" s="2"/>
-      <c r="L1000" s="3"/>
-      <c r="M1000" s="3"/>
-      <c r="N1000" s="1"/>
-      <c r="O1000" s="1"/>
-      <c r="P1000" s="1"/>
-      <c r="Q1000" s="1"/>
-      <c r="R1000" s="1"/>
-      <c r="S1000" s="1"/>
-      <c r="T1000" s="1"/>
-      <c r="U1000" s="1"/>
-      <c r="V1000" s="1"/>
-      <c r="W1000" s="1"/>
-      <c r="X1000" s="1"/>
-      <c r="Y1000" s="1"/>
-      <c r="Z1000" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C57:C1000 C33:C45 C1:C31" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C56:C999 C32:C44 C1:C30" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E33:E1000 E1:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E32:E999 E1:E30" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F33:F1000 F1:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F32:F999 F1:F30" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33:H1000 H1:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H32:H999 H1:H30" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28800,13 +28756,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28837,10 +28793,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
change column metadata value
</commit_message>
<xml_diff>
--- a/data-raw/metadata/yuba_catch_metadata.xlsx
+++ b/data-raw/metadata/yuba_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inigo\Projects\jpe-yuba-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DF55D3-A3A6-4EFA-944D-330393248467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B116BE-4DB4-4A8E-9CAA-757BF9602B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54495" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37350" yWindow="5580" windowWidth="27975" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>fishOrigin</t>
   </si>
   <si>
-    <t>ActualCount</t>
-  </si>
-  <si>
     <t>millimeter</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Foreign Key to the CAMP Release table</t>
+  </si>
+  <si>
+    <t>actualCount</t>
   </si>
 </sst>
 </file>
@@ -533,8 +533,8 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -705,7 +705,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="12">
@@ -733,7 +733,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -771,7 +771,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -809,7 +809,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -885,7 +885,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -920,10 +920,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -961,7 +961,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -999,7 +999,7 @@
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1090,7 +1090,7 @@
         <v>23</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>25</v>
@@ -1138,7 +1138,7 @@
         <v>23</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>30</v>
@@ -1186,7 +1186,7 @@
         <v>23</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>25</v>
@@ -1216,10 +1216,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -28837,7 +28837,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>37</v>

</xml_diff>